<commit_message>
Chnages Done in JSY Report
Total row updation with district data and Heading changes done.
</commit_message>
<xml_diff>
--- a/OutputReports/DHIS2 Reports/HTML Reports/UPHMIS/Final Updated Reports/MPR--Vector Borne Disease Control Program (Dengue)/MPR--Vector Borne Disease Control Program (Dengue).xlsx
+++ b/OutputReports/DHIS2 Reports/HTML Reports/UPHMIS/Final Updated Reports/MPR--Vector Borne Disease Control Program (Dengue)/MPR--Vector Borne Disease Control Program (Dengue).xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="87">
   <si>
     <t>Reporting Month:</t>
   </si>
@@ -33,9 +33,6 @@
   </si>
   <si>
     <t>Monthly</t>
-  </si>
-  <si>
-    <t>Cumu.</t>
   </si>
   <si>
     <t>Report Name</t>
@@ -1089,7 +1086,6 @@
     <xf numFmtId="2" fontId="25" fillId="34" borderId="10" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="10" xfId="47" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="35" borderId="10" xfId="47" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1098,43 +1094,46 @@
     <xf numFmtId="2" fontId="25" fillId="34" borderId="10" xfId="47" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="34" borderId="10" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="10" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="10" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="10" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="34" borderId="10" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="34" borderId="10" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="10" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="10" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="34" borderId="15" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="34" borderId="16" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="10" xfId="47" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="34" borderId="0" xfId="47" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="34" borderId="10" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="34" borderId="10" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="10" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="34" borderId="10" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="34" borderId="15" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="34" borderId="16" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="10" xfId="47" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="34" borderId="10" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="34" borderId="10" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="34" borderId="10" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="34" borderId="10" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="34" borderId="10" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1535,70 +1534,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AP10"/>
+  <dimension ref="A1:AF9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="AM9" sqref="AM9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:42" ht="15.75">
-      <c r="A1" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
-      <c r="O1" s="34"/>
-      <c r="P1" s="34"/>
-      <c r="Q1" s="34"/>
-      <c r="R1" s="34"/>
-      <c r="S1" s="34"/>
-      <c r="T1" s="34"/>
-      <c r="U1" s="34"/>
-      <c r="V1" s="34"/>
-      <c r="W1" s="34"/>
-      <c r="X1" s="34"/>
-      <c r="Y1" s="34"/>
-      <c r="Z1" s="34"/>
-      <c r="AA1" s="34"/>
-      <c r="AB1" s="34"/>
-      <c r="AC1" s="34"/>
-      <c r="AD1" s="34"/>
-      <c r="AE1" s="34"/>
-      <c r="AF1" s="34"/>
-      <c r="AG1" s="34"/>
-      <c r="AH1" s="34"/>
-      <c r="AI1" s="34"/>
-      <c r="AJ1" s="34"/>
-      <c r="AK1" s="34"/>
-      <c r="AL1" s="34"/>
-      <c r="AM1" s="34"/>
-      <c r="AN1" s="34"/>
-      <c r="AO1" s="34"/>
-      <c r="AP1" s="34"/>
-    </row>
-    <row r="2" spans="1:42" s="30" customFormat="1" ht="15.75">
-      <c r="A2" s="39" t="s">
+    <row r="1" spans="1:32" ht="15.75">
+      <c r="A1" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
+      <c r="N1" s="44"/>
+      <c r="O1" s="44"/>
+      <c r="P1" s="44"/>
+      <c r="Q1" s="44"/>
+      <c r="R1" s="44"/>
+      <c r="S1" s="44"/>
+      <c r="T1" s="44"/>
+      <c r="U1" s="44"/>
+      <c r="V1" s="44"/>
+      <c r="W1" s="44"/>
+      <c r="X1" s="44"/>
+      <c r="Y1" s="44"/>
+      <c r="Z1" s="44"/>
+      <c r="AA1" s="44"/>
+      <c r="AB1" s="44"/>
+      <c r="AC1" s="44"/>
+      <c r="AD1" s="44"/>
+      <c r="AE1" s="44"/>
+      <c r="AF1" s="44"/>
+    </row>
+    <row r="2" spans="1:32" s="29" customFormat="1" ht="15.75">
+      <c r="A2" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="25"/>
       <c r="H2" s="25"/>
       <c r="I2" s="25"/>
       <c r="J2" s="25"/>
@@ -1624,192 +1613,154 @@
       <c r="AD2" s="25"/>
       <c r="AE2" s="25"/>
       <c r="AF2" s="25"/>
-      <c r="AG2" s="25"/>
-      <c r="AH2" s="25"/>
-      <c r="AI2" s="25"/>
-      <c r="AJ2" s="25"/>
-      <c r="AK2" s="25"/>
-      <c r="AL2" s="25"/>
-      <c r="AM2" s="25"/>
-      <c r="AN2" s="25"/>
-      <c r="AO2" s="25"/>
-      <c r="AP2" s="25"/>
-    </row>
-    <row r="3" spans="1:42" s="30" customFormat="1" ht="18.75">
-      <c r="A3" s="41" t="s">
+    </row>
+    <row r="3" spans="1:32" s="29" customFormat="1" ht="18.75">
+      <c r="A3" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="43" t="s">
+      <c r="B3" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="43" t="s">
+      <c r="C3" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="43" t="s">
+      <c r="D3" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="44" t="s">
+      <c r="E3" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="38"/>
+      <c r="M3" s="38"/>
+      <c r="N3" s="38"/>
+      <c r="O3" s="38"/>
+      <c r="P3" s="38"/>
+      <c r="Q3" s="38"/>
+      <c r="R3" s="38"/>
+      <c r="S3" s="38"/>
+      <c r="T3" s="38"/>
+      <c r="U3" s="38"/>
+      <c r="V3" s="38"/>
+      <c r="W3" s="38"/>
+      <c r="X3" s="38"/>
+      <c r="Y3" s="38"/>
+      <c r="Z3" s="38"/>
+      <c r="AA3" s="38"/>
+      <c r="AB3" s="38"/>
+      <c r="AC3" s="38"/>
+      <c r="AD3" s="38"/>
+      <c r="AE3" s="38"/>
+      <c r="AF3" s="38"/>
+    </row>
+    <row r="4" spans="1:32" s="29" customFormat="1">
+      <c r="A4" s="43"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
-      <c r="K3" s="44"/>
-      <c r="L3" s="44"/>
-      <c r="M3" s="44"/>
-      <c r="N3" s="44"/>
-      <c r="O3" s="44"/>
-      <c r="P3" s="44"/>
-      <c r="Q3" s="44"/>
-      <c r="R3" s="44"/>
-      <c r="S3" s="44"/>
-      <c r="T3" s="44"/>
-      <c r="U3" s="44"/>
-      <c r="V3" s="44"/>
-      <c r="W3" s="44"/>
-      <c r="X3" s="44"/>
-      <c r="Y3" s="44"/>
-      <c r="Z3" s="44"/>
-      <c r="AA3" s="44"/>
-      <c r="AB3" s="44"/>
-      <c r="AC3" s="44"/>
-      <c r="AD3" s="44"/>
-      <c r="AE3" s="44"/>
-      <c r="AF3" s="44"/>
-      <c r="AG3" s="44"/>
-      <c r="AH3" s="44"/>
-      <c r="AI3" s="44"/>
-      <c r="AJ3" s="44"/>
-      <c r="AK3" s="44"/>
-      <c r="AL3" s="44"/>
-      <c r="AM3" s="44"/>
-      <c r="AN3" s="44"/>
-      <c r="AO3" s="44"/>
-      <c r="AP3" s="44"/>
-    </row>
-    <row r="4" spans="1:42" s="30" customFormat="1">
-      <c r="A4" s="41"/>
-      <c r="B4" s="43"/>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="45" t="s">
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="39"/>
+      <c r="K4" s="39"/>
+      <c r="L4" s="39"/>
+      <c r="M4" s="39"/>
+      <c r="N4" s="39"/>
+      <c r="O4" s="39"/>
+      <c r="P4" s="39"/>
+      <c r="Q4" s="39"/>
+      <c r="R4" s="39"/>
+      <c r="S4" s="39"/>
+      <c r="T4" s="39"/>
+      <c r="U4" s="39"/>
+      <c r="V4" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
-      <c r="K4" s="45"/>
-      <c r="L4" s="45"/>
-      <c r="M4" s="45"/>
-      <c r="N4" s="45"/>
-      <c r="O4" s="45"/>
-      <c r="P4" s="45"/>
-      <c r="Q4" s="45"/>
-      <c r="R4" s="45"/>
-      <c r="S4" s="45"/>
-      <c r="T4" s="45"/>
-      <c r="U4" s="45"/>
-      <c r="V4" s="45"/>
-      <c r="W4" s="45"/>
-      <c r="X4" s="45"/>
-      <c r="Y4" s="45"/>
-      <c r="Z4" s="45"/>
-      <c r="AA4" s="46" t="s">
+      <c r="W4" s="40"/>
+      <c r="X4" s="40"/>
+      <c r="Y4" s="40"/>
+      <c r="Z4" s="40"/>
+      <c r="AA4" s="40"/>
+      <c r="AB4" s="40"/>
+      <c r="AC4" s="40"/>
+      <c r="AD4" s="40"/>
+      <c r="AE4" s="40"/>
+      <c r="AF4" s="40"/>
+    </row>
+    <row r="5" spans="1:32" s="29" customFormat="1">
+      <c r="A5" s="43"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="AB4" s="46"/>
-      <c r="AC4" s="46"/>
-      <c r="AD4" s="46"/>
-      <c r="AE4" s="46"/>
-      <c r="AF4" s="46"/>
-      <c r="AG4" s="46"/>
-      <c r="AH4" s="46"/>
-      <c r="AI4" s="46"/>
-      <c r="AJ4" s="46"/>
-      <c r="AK4" s="46"/>
-      <c r="AL4" s="46"/>
-      <c r="AM4" s="46"/>
-      <c r="AN4" s="46"/>
-      <c r="AO4" s="46"/>
-      <c r="AP4" s="46"/>
-    </row>
-    <row r="5" spans="1:42" s="30" customFormat="1">
-      <c r="A5" s="41"/>
-      <c r="B5" s="43"/>
-      <c r="C5" s="43"/>
-      <c r="D5" s="43"/>
-      <c r="E5" s="37" t="s">
+      <c r="F5" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="F5" s="37"/>
-      <c r="G5" s="42" t="s">
+      <c r="G5" s="36"/>
+      <c r="H5" s="36"/>
+      <c r="I5" s="36"/>
+      <c r="J5" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="H5" s="42"/>
-      <c r="I5" s="42"/>
-      <c r="J5" s="42"/>
-      <c r="K5" s="42" t="s">
+      <c r="K5" s="36"/>
+      <c r="L5" s="36"/>
+      <c r="M5" s="36"/>
+      <c r="N5" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="L5" s="42"/>
-      <c r="M5" s="42"/>
-      <c r="N5" s="42"/>
-      <c r="O5" s="42" t="s">
+      <c r="O5" s="36"/>
+      <c r="P5" s="36"/>
+      <c r="Q5" s="36"/>
+      <c r="R5" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="P5" s="42"/>
-      <c r="Q5" s="42"/>
-      <c r="R5" s="42"/>
-      <c r="S5" s="37" t="s">
+      <c r="S5" s="35"/>
+      <c r="T5" s="35"/>
+      <c r="U5" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="T5" s="37"/>
-      <c r="U5" s="37"/>
-      <c r="V5" s="37"/>
-      <c r="W5" s="37"/>
-      <c r="X5" s="37"/>
-      <c r="Y5" s="37" t="s">
+      <c r="V5" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="Z5" s="37"/>
-      <c r="AA5" s="37" t="s">
+      <c r="W5" s="46" t="s">
         <v>44</v>
       </c>
-      <c r="AB5" s="37"/>
-      <c r="AC5" s="38" t="s">
+      <c r="X5" s="46"/>
+      <c r="Y5" s="46"/>
+      <c r="Z5" s="45" t="s">
         <v>45</v>
       </c>
-      <c r="AD5" s="38"/>
-      <c r="AE5" s="38"/>
-      <c r="AF5" s="36" t="s">
+      <c r="AA5" s="45"/>
+      <c r="AB5" s="45"/>
+      <c r="AC5" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD5" s="45"/>
+      <c r="AE5" s="45"/>
+      <c r="AF5" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="AG5" s="36"/>
-      <c r="AH5" s="36"/>
-      <c r="AI5" s="36" t="s">
-        <v>42</v>
-      </c>
-      <c r="AJ5" s="36"/>
-      <c r="AK5" s="36"/>
-      <c r="AL5" s="36"/>
-      <c r="AM5" s="36"/>
-      <c r="AN5" s="36"/>
-      <c r="AO5" s="37" t="s">
+    </row>
+    <row r="6" spans="1:32" s="29" customFormat="1" ht="63.75">
+      <c r="A6" s="43"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="AP5" s="37"/>
-    </row>
-    <row r="6" spans="1:42" s="30" customFormat="1" ht="63.75">
-      <c r="A6" s="41"/>
-      <c r="B6" s="43"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
       <c r="G6" s="26" t="s">
         <v>48</v>
       </c>
@@ -1820,7 +1771,7 @@
         <v>50</v>
       </c>
       <c r="J6" s="26" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="K6" s="26" t="s">
         <v>48</v>
@@ -1832,7 +1783,7 @@
         <v>50</v>
       </c>
       <c r="N6" s="26" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="O6" s="26" t="s">
         <v>48</v>
@@ -1843,428 +1794,286 @@
       <c r="Q6" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="R6" s="26" t="s">
+      <c r="R6" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="S6" s="37" t="s">
+      <c r="S6" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="T6" s="37"/>
-      <c r="U6" s="37" t="s">
+      <c r="T6" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="V6" s="37"/>
-      <c r="W6" s="37" t="s">
+      <c r="U6" s="35"/>
+      <c r="V6" s="35"/>
+      <c r="W6" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="X6" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="X6" s="37"/>
-      <c r="Y6" s="37"/>
-      <c r="Z6" s="37"/>
-      <c r="AA6" s="37"/>
-      <c r="AB6" s="37"/>
-      <c r="AC6" s="26" t="s">
-        <v>39</v>
-      </c>
-      <c r="AD6" s="26" t="s">
+      <c r="Y6" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z6" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="AE6" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="AF6" s="26" t="s">
+      <c r="AA6" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB6" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC6" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="AG6" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="AH6" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="AI6" s="37" t="s">
+      <c r="AD6" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="AJ6" s="37"/>
-      <c r="AK6" s="37" t="s">
+      <c r="AE6" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="AL6" s="37"/>
-      <c r="AM6" s="37" t="s">
+      <c r="AF6" s="35"/>
+    </row>
+    <row r="7" spans="1:32" ht="17.25">
+      <c r="A7" s="43"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="33">
+        <v>3.1</v>
+      </c>
+      <c r="F7" s="27">
+        <v>3.2</v>
+      </c>
+      <c r="G7" s="27">
+        <v>3.3</v>
+      </c>
+      <c r="H7" s="27">
+        <v>3.4</v>
+      </c>
+      <c r="I7" s="27">
+        <v>3.5</v>
+      </c>
+      <c r="J7" s="27">
+        <v>3.6</v>
+      </c>
+      <c r="K7" s="27">
+        <v>3.7</v>
+      </c>
+      <c r="L7" s="27">
+        <v>3.8</v>
+      </c>
+      <c r="M7" s="27">
+        <v>3.9</v>
+      </c>
+      <c r="N7" s="28">
+        <v>3.1</v>
+      </c>
+      <c r="O7" s="28">
+        <v>3.11</v>
+      </c>
+      <c r="P7" s="28">
+        <v>3.12</v>
+      </c>
+      <c r="Q7" s="28">
+        <v>3.13</v>
+      </c>
+      <c r="R7" s="32">
+        <v>3.14</v>
+      </c>
+      <c r="S7" s="32">
+        <v>3.15</v>
+      </c>
+      <c r="T7" s="32">
+        <v>3.16</v>
+      </c>
+      <c r="U7" s="33">
+        <v>3.17</v>
+      </c>
+      <c r="V7" s="33">
+        <v>3.18</v>
+      </c>
+      <c r="W7" s="28">
+        <v>3.2</v>
+      </c>
+      <c r="X7" s="28">
+        <v>3.21</v>
+      </c>
+      <c r="Y7" s="28">
+        <v>3.22</v>
+      </c>
+      <c r="Z7" s="28">
+        <v>3.24</v>
+      </c>
+      <c r="AA7" s="28">
+        <v>3.25</v>
+      </c>
+      <c r="AB7" s="28">
+        <v>3.26</v>
+      </c>
+      <c r="AC7" s="32">
+        <v>3.27</v>
+      </c>
+      <c r="AD7" s="32">
+        <v>3.28</v>
+      </c>
+      <c r="AE7" s="32">
+        <v>3.29</v>
+      </c>
+      <c r="AF7" s="33">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" s="30" customFormat="1" ht="57" customHeight="1">
+      <c r="A8" s="24">
+        <v>1</v>
+      </c>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="AN6" s="37"/>
-      <c r="AO6" s="37"/>
-      <c r="AP6" s="37"/>
-    </row>
-    <row r="7" spans="1:42" ht="17.25">
-      <c r="A7" s="41"/>
-      <c r="B7" s="43"/>
-      <c r="C7" s="43"/>
-      <c r="D7" s="43"/>
-      <c r="E7" s="35">
-        <v>3.1</v>
-      </c>
-      <c r="F7" s="35"/>
-      <c r="G7" s="27">
-        <v>3.2</v>
-      </c>
-      <c r="H7" s="27">
-        <v>3.3</v>
-      </c>
-      <c r="I7" s="27">
-        <v>3.4</v>
-      </c>
-      <c r="J7" s="27">
-        <v>3.5</v>
-      </c>
-      <c r="K7" s="27">
-        <v>3.6</v>
-      </c>
-      <c r="L7" s="27">
-        <v>3.7</v>
-      </c>
-      <c r="M7" s="27">
-        <v>3.8</v>
-      </c>
-      <c r="N7" s="27">
-        <v>3.9</v>
-      </c>
-      <c r="O7" s="28">
-        <v>3.1</v>
-      </c>
-      <c r="P7" s="28">
-        <v>3.11</v>
-      </c>
-      <c r="Q7" s="28">
-        <v>3.12</v>
-      </c>
-      <c r="R7" s="28">
-        <v>3.13</v>
-      </c>
-      <c r="S7" s="33">
-        <v>3.14</v>
-      </c>
-      <c r="T7" s="33"/>
-      <c r="U7" s="33">
-        <v>3.15</v>
-      </c>
-      <c r="V7" s="33"/>
-      <c r="W7" s="33">
-        <v>3.16</v>
-      </c>
-      <c r="X7" s="33"/>
-      <c r="Y7" s="35">
-        <v>3.17</v>
-      </c>
-      <c r="Z7" s="35"/>
-      <c r="AA7" s="35">
-        <v>3.18</v>
-      </c>
-      <c r="AB7" s="35"/>
-      <c r="AC7" s="28">
-        <v>3.2</v>
-      </c>
-      <c r="AD7" s="28">
-        <v>3.21</v>
-      </c>
-      <c r="AE7" s="28">
-        <v>3.22</v>
-      </c>
-      <c r="AF7" s="28">
-        <v>3.24</v>
-      </c>
-      <c r="AG7" s="28">
-        <v>3.25</v>
-      </c>
-      <c r="AH7" s="28">
-        <v>3.26</v>
-      </c>
-      <c r="AI7" s="33">
-        <v>3.27</v>
-      </c>
-      <c r="AJ7" s="33"/>
-      <c r="AK7" s="33">
-        <v>3.28</v>
-      </c>
-      <c r="AL7" s="33"/>
-      <c r="AM7" s="33">
-        <v>3.29</v>
-      </c>
-      <c r="AN7" s="33"/>
-      <c r="AO7" s="35">
-        <v>3.3</v>
-      </c>
-      <c r="AP7" s="35"/>
-    </row>
-    <row r="8" spans="1:42">
-      <c r="A8" s="41"/>
-      <c r="B8" s="43"/>
-      <c r="C8" s="43"/>
-      <c r="D8" s="43"/>
-      <c r="E8" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="F8" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="G8" s="29"/>
-      <c r="H8" s="29"/>
-      <c r="I8" s="29"/>
-      <c r="J8" s="29"/>
-      <c r="K8" s="29"/>
-      <c r="L8" s="29"/>
-      <c r="M8" s="29"/>
-      <c r="N8" s="29"/>
-      <c r="O8" s="29"/>
-      <c r="P8" s="29"/>
-      <c r="Q8" s="29"/>
-      <c r="R8" s="29"/>
-      <c r="S8" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="T8" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="U8" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="V8" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="W8" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="X8" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="Y8" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="Z8" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="AA8" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="AB8" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="AC8" s="29"/>
-      <c r="AD8" s="29"/>
-      <c r="AE8" s="29"/>
-      <c r="AF8" s="29"/>
-      <c r="AG8" s="29"/>
-      <c r="AH8" s="29"/>
-      <c r="AI8" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="AJ8" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="AK8" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="AL8" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="AM8" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="AN8" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="AO8" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="AP8" s="29" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:42" s="31" customFormat="1" ht="57" customHeight="1">
+      <c r="F8" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="G8" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="H8" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="I8" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="J8" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="K8" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="L8" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="M8" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="N8" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="O8" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="P8" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q8" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="R8" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="S8" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="T8" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="U8" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="V8" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="W8" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="X8" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="Y8" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z8" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA8" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="AB8" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC8" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="AD8" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE8" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="AF8" s="31" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32" s="30" customFormat="1" ht="45.75" customHeight="1">
       <c r="A9" s="24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B9" s="24"/>
       <c r="C9" s="24"/>
       <c r="D9" s="24"/>
-      <c r="E9" s="32" t="s">
-        <v>60</v>
-      </c>
+      <c r="E9" s="24"/>
       <c r="F9" s="24"/>
-      <c r="G9" s="32" t="s">
-        <v>61</v>
-      </c>
-      <c r="H9" s="32" t="s">
-        <v>62</v>
-      </c>
-      <c r="I9" s="32" t="s">
-        <v>63</v>
-      </c>
-      <c r="J9" s="32" t="s">
-        <v>64</v>
-      </c>
-      <c r="K9" s="32" t="s">
-        <v>65</v>
-      </c>
-      <c r="L9" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="M9" s="32" t="s">
-        <v>67</v>
-      </c>
-      <c r="N9" s="32" t="s">
-        <v>68</v>
-      </c>
-      <c r="O9" s="32" t="s">
-        <v>69</v>
-      </c>
-      <c r="P9" s="32" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q9" s="32" t="s">
-        <v>71</v>
-      </c>
-      <c r="R9" s="32" t="s">
-        <v>72</v>
-      </c>
-      <c r="S9" s="32" t="s">
-        <v>73</v>
-      </c>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="24"/>
+      <c r="M9" s="24"/>
+      <c r="N9" s="24"/>
+      <c r="O9" s="24"/>
+      <c r="P9" s="24"/>
+      <c r="Q9" s="24"/>
+      <c r="R9" s="24"/>
+      <c r="S9" s="24"/>
       <c r="T9" s="24"/>
-      <c r="U9" s="32" t="s">
-        <v>74</v>
-      </c>
+      <c r="U9" s="24"/>
       <c r="V9" s="24"/>
-      <c r="W9" s="32" t="s">
-        <v>75</v>
-      </c>
+      <c r="W9" s="24"/>
       <c r="X9" s="24"/>
-      <c r="Y9" s="32" t="s">
-        <v>76</v>
-      </c>
+      <c r="Y9" s="24"/>
       <c r="Z9" s="24"/>
-      <c r="AA9" s="32" t="s">
-        <v>77</v>
-      </c>
+      <c r="AA9" s="24"/>
       <c r="AB9" s="24"/>
-      <c r="AC9" s="32" t="s">
-        <v>78</v>
-      </c>
-      <c r="AD9" s="32" t="s">
-        <v>79</v>
-      </c>
-      <c r="AE9" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="AF9" s="32" t="s">
-        <v>81</v>
-      </c>
-      <c r="AG9" s="32" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH9" s="32" t="s">
-        <v>83</v>
-      </c>
-      <c r="AI9" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="AJ9" s="24"/>
-      <c r="AK9" s="32" t="s">
-        <v>85</v>
-      </c>
-      <c r="AL9" s="24"/>
-      <c r="AM9" s="32" t="s">
-        <v>86</v>
-      </c>
-      <c r="AN9" s="24"/>
-      <c r="AO9" s="32" t="s">
-        <v>87</v>
-      </c>
-      <c r="AP9" s="24"/>
-    </row>
-    <row r="10" spans="1:42" s="31" customFormat="1" ht="45.75" customHeight="1">
-      <c r="A10" s="24">
-        <v>2</v>
-      </c>
-      <c r="B10" s="24"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="24"/>
-      <c r="J10" s="24"/>
-      <c r="K10" s="24"/>
-      <c r="L10" s="24"/>
-      <c r="M10" s="24"/>
-      <c r="N10" s="24"/>
-      <c r="O10" s="24"/>
-      <c r="P10" s="24"/>
-      <c r="Q10" s="24"/>
-      <c r="R10" s="24"/>
-      <c r="S10" s="24"/>
-      <c r="T10" s="24"/>
-      <c r="U10" s="24"/>
-      <c r="V10" s="24"/>
-      <c r="W10" s="24"/>
-      <c r="X10" s="24"/>
-      <c r="Y10" s="24"/>
-      <c r="Z10" s="24"/>
-      <c r="AA10" s="24"/>
-      <c r="AB10" s="24"/>
-      <c r="AC10" s="24"/>
-      <c r="AD10" s="24"/>
-      <c r="AE10" s="24"/>
-      <c r="AF10" s="24"/>
-      <c r="AG10" s="24"/>
-      <c r="AH10" s="24"/>
-      <c r="AI10" s="24"/>
-      <c r="AJ10" s="24"/>
-      <c r="AK10" s="24"/>
-      <c r="AL10" s="24"/>
-      <c r="AM10" s="24"/>
-      <c r="AN10" s="24"/>
-      <c r="AO10" s="24"/>
-      <c r="AP10" s="24"/>
+      <c r="AC9" s="24"/>
+      <c r="AD9" s="24"/>
+      <c r="AE9" s="24"/>
+      <c r="AF9" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="36">
-    <mergeCell ref="AO7:AP7"/>
-    <mergeCell ref="AK6:AL6"/>
-    <mergeCell ref="AM6:AN6"/>
-    <mergeCell ref="K5:N5"/>
-    <mergeCell ref="B3:B8"/>
-    <mergeCell ref="C3:C8"/>
-    <mergeCell ref="D3:D8"/>
-    <mergeCell ref="E3:AP3"/>
-    <mergeCell ref="E4:Z4"/>
-    <mergeCell ref="AA4:AP4"/>
-    <mergeCell ref="E5:F6"/>
-    <mergeCell ref="G5:J5"/>
-    <mergeCell ref="O5:R5"/>
-    <mergeCell ref="AA5:AB6"/>
-    <mergeCell ref="S5:X5"/>
-    <mergeCell ref="W6:X6"/>
-    <mergeCell ref="AI7:AJ7"/>
-    <mergeCell ref="AI6:AJ6"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A3:A8"/>
-    <mergeCell ref="AK7:AL7"/>
-    <mergeCell ref="AM7:AN7"/>
-    <mergeCell ref="A1:AP1"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="S7:T7"/>
-    <mergeCell ref="U7:V7"/>
-    <mergeCell ref="W7:X7"/>
-    <mergeCell ref="Y7:Z7"/>
-    <mergeCell ref="AA7:AB7"/>
-    <mergeCell ref="AF5:AH5"/>
-    <mergeCell ref="AI5:AN5"/>
-    <mergeCell ref="AO5:AP6"/>
-    <mergeCell ref="S6:T6"/>
-    <mergeCell ref="U6:V6"/>
-    <mergeCell ref="Y5:Z6"/>
+  <mergeCells count="20">
+    <mergeCell ref="A1:AF1"/>
+    <mergeCell ref="Z5:AB5"/>
     <mergeCell ref="AC5:AE5"/>
+    <mergeCell ref="AF5:AF6"/>
+    <mergeCell ref="U5:U6"/>
+    <mergeCell ref="W5:Y5"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="J5:M5"/>
+    <mergeCell ref="B3:B7"/>
+    <mergeCell ref="C3:C7"/>
+    <mergeCell ref="D3:D7"/>
+    <mergeCell ref="E3:AF3"/>
+    <mergeCell ref="E4:U4"/>
+    <mergeCell ref="V4:AF4"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="N5:Q5"/>
+    <mergeCell ref="V5:V6"/>
+    <mergeCell ref="R5:T5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2288,49 +2097,49 @@
   <sheetData>
     <row r="1" spans="1:3" ht="38.25" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C1" s="3"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>8</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>9</v>
       </c>
       <c r="C2" s="6"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="49" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>10</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>11</v>
       </c>
       <c r="C3" s="6"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="50"/>
       <c r="B4" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" s="6"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="50"/>
       <c r="B5" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" s="6"/>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="51"/>
       <c r="B6" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" s="6"/>
     </row>
@@ -2341,47 +2150,47 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="10" t="s">
         <v>15</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>16</v>
       </c>
       <c r="C8" s="11"/>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="53" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9" s="6"/>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="54"/>
       <c r="B10" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" s="6"/>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="54"/>
       <c r="B11" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11" s="6"/>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="54"/>
       <c r="B12" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C12" s="6"/>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="55"/>
       <c r="B13" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C13" s="6"/>
     </row>
@@ -2392,21 +2201,21 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="C15" s="14" t="s">
         <v>23</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="16" t="s">
         <v>25</v>
-      </c>
-      <c r="B16" s="16" t="s">
-        <v>26</v>
       </c>
       <c r="C16" s="17" t="s">
         <v>5</v>
@@ -2429,33 +2238,33 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="18" t="s">
         <v>27</v>
-      </c>
-      <c r="B20" s="18" t="s">
-        <v>28</v>
       </c>
       <c r="C20" s="19"/>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="20"/>
       <c r="B21" s="18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C21" s="19"/>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="61" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C22" s="19"/>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="61"/>
       <c r="B23" s="21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C23" s="6"/>
     </row>
@@ -2471,19 +2280,19 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" s="10" t="s">
         <v>31</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>32</v>
       </c>
       <c r="C26" s="18"/>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="47" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C27" s="18"/>
     </row>

</xml_diff>